<commit_message>
add 16 moon and 5 dwarf planet (cover all bodies whose diameter > 950km)
</commit_message>
<xml_diff>
--- a/solar_system.xlsx
+++ b/solar_system.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
   <si>
     <t>名字</t>
   </si>
@@ -96,14 +96,6 @@
   </si>
   <si>
     <t>轨道半径（km）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>公转周期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>87.9691天</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -139,18 +131,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>224.7天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>365.242天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>686.98天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>7.785472</t>
     </r>
@@ -164,14 +144,6 @@
       </rPr>
       <t>×10^8</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10832.327天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4329.557天</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -201,30 +173,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>30667.485天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>4.503443661</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>×10^9</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>60327.624天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>1.0820893</t>
     </r>
@@ -284,6 +232,298 @@
       </rPr>
       <t>×10^9</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>月球 Moon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.349×10^22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.84403×10^5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.9319×10^22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.217×10^5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公转周期（天）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木卫一 Io 艾奥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木卫二 Europa 欧罗巴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木卫三 Ganymede 盖尼米德</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.8×10^22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.4819×10^23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0704×10^6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木卫四 Callisto 卡里斯托</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.08×10^23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.88×10^6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;=1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>4.503443661</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>×10^9</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.91352×10^9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.473×10^22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冥王星 Pluto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阋神星 Eris</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>离心率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸟神星 Makemake</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.66×10^22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4×10^21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.78×10^9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>妊神星 Haumea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2×10^21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>谷神星 Ceres</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.43×10^20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.452×10^9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1410698×10^8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>土卫三 Tethys</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.774×10^5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>土卫四 Dione</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>土卫五 Rhea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.306518×10^21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.27108×10^5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>土卫六 Titan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.3452×10^23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.221833×10^6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>土卫八 Lapetus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.5613×10^6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天卫一 Ariel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.909×10^5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天卫二 Umbriel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.27×10^21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.663×10^5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天卫三 Titania</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.526×10^21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天卫四 Oberon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.014×10^21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.55×10^5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海卫一 Triton</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.147×10^22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冥卫一 Charon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.52×10^21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.012×10^10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.71034×10^5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.17449×10^20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.94619×10^5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.096×10^21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.88×10^21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小周期需要小的dt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.353×10^21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.3591×10^5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.8352×10^5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.974×10^4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -680,25 +920,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G11"/>
+  <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,16 +952,19 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -732,7 +975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -743,19 +986,22 @@
         <v>4878</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1">
         <v>47.89</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
+      <c r="F4" s="1">
+        <v>87.969099999999997</v>
       </c>
       <c r="G4" s="1">
         <v>7.0048700000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H4" s="1">
+        <v>0.20563000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -766,19 +1012,22 @@
         <v>12103</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1">
         <v>35.03</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>28</v>
+      <c r="F5" s="1">
+        <v>224.7</v>
       </c>
       <c r="G5" s="1">
         <v>3.395</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H5" s="1">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -789,19 +1038,22 @@
         <v>12756</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1">
         <v>29.783000000000001</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>29</v>
+      <c r="F6" s="1">
+        <v>365.24200000000002</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H6" s="1">
+        <v>1.67E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -812,19 +1064,22 @@
         <v>6794</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>24.131</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
+      <c r="F7" s="1">
+        <v>686.98</v>
       </c>
       <c r="G7" s="1">
         <v>1.8506100000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H7" s="1">
+        <v>9.3412330000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -835,19 +1090,22 @@
         <v>142984</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1">
         <v>13.07</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>33</v>
+      <c r="F8" s="1">
+        <v>4329.5569999999998</v>
       </c>
       <c r="G8" s="1">
         <v>1.3052999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H8" s="1">
+        <v>4.8774999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -858,19 +1116,22 @@
         <v>120540</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1">
         <v>9.69</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>32</v>
+      <c r="F9" s="1">
+        <v>10832.326999999999</v>
       </c>
       <c r="G9" s="1">
         <v>2.4852400000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H9" s="1">
+        <v>5.5723218999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -881,19 +1142,22 @@
         <v>51118</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1">
         <v>6.8353000000000002</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>35</v>
+      <c r="F10" s="1">
+        <v>30667.485000000001</v>
       </c>
       <c r="G10" s="1">
         <v>0.77255600000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H10" s="1">
+        <v>4.4405585999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -904,16 +1168,575 @@
         <v>49532</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1">
         <v>5.4778000000000002</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>37</v>
+      <c r="F11" s="4">
+        <v>60327.624000000003</v>
       </c>
       <c r="G11" s="1">
         <v>1.7679750000000001</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.1214269000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2370</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4.7488999999999999</v>
+      </c>
+      <c r="F13" s="1">
+        <v>90581</v>
+      </c>
+      <c r="G13" s="1">
+        <v>17.1449</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.24904999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2326</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3.4630000000000001</v>
+      </c>
+      <c r="F14" s="1">
+        <v>203600</v>
+      </c>
+      <c r="G14" s="1">
+        <v>44.186999999999998</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.44177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1600</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="1">
+        <v>4.4189999999999996</v>
+      </c>
+      <c r="F15" s="1">
+        <v>113183</v>
+      </c>
+      <c r="G15" s="1">
+        <v>28.96</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1436</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4.484</v>
+      </c>
+      <c r="F16" s="1">
+        <v>103468</v>
+      </c>
+      <c r="G16" s="1">
+        <v>28.22</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.19500999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="1">
+        <v>950</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="1">
+        <v>17.882000000000001</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1680.5</v>
+      </c>
+      <c r="G17" s="1">
+        <v>10.585000000000001</v>
+      </c>
+      <c r="H17" s="1">
+        <v>7.5705099999999997E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3476</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.0229999999999999</v>
+      </c>
+      <c r="F20" s="1">
+        <v>27.32</v>
+      </c>
+      <c r="G20" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="H20" s="1">
+        <v>5.4899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3637.4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="1">
+        <v>17.334</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.7689999999999999</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="H21" s="1">
+        <v>4.1000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3138</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="1">
+        <v>13.741</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3.5510000000000002</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="1">
+        <v>9.4000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5262</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="1">
+        <v>10.88</v>
+      </c>
+      <c r="F23" s="1">
+        <v>7</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H23" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4820</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="1">
+        <v>8.1829999999999998</v>
+      </c>
+      <c r="F24" s="1">
+        <v>16.7</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H24" s="1">
+        <v>7.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1062</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="1">
+        <v>11.349</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1.8877999999999999</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1118</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="1">
+        <v>10.028</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2.7368999999999999</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1532</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="1">
+        <v>8.484</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4.5182000000000002</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1.2583E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="1">
+        <v>5150</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="1">
+        <v>5.5724</v>
+      </c>
+      <c r="F28" s="1">
+        <v>15.945399999999999</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2.92E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1460</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="1">
+        <v>3.2646999999999999</v>
+      </c>
+      <c r="F29" s="1">
+        <v>79.33</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1157.8</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="1">
+        <v>5.5090000000000003</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2.52</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="H30" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1169.4000000000001</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4.673</v>
+      </c>
+      <c r="F31" s="1">
+        <v>4.1440000000000001</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="H31" s="1">
+        <v>3.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1576.8</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="1">
+        <v>3.641</v>
+      </c>
+      <c r="F32" s="1">
+        <v>8.7059999999999995</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1522.8</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3.1520000000000001</v>
+      </c>
+      <c r="F33" s="1">
+        <v>13.462999999999999</v>
+      </c>
+      <c r="G33" s="1">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2706.8</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4.3929999999999998</v>
+      </c>
+      <c r="F34" s="1">
+        <v>5.8769999999999998</v>
+      </c>
+      <c r="G34" s="1">
+        <v>157.34</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1207</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.2243</v>
+      </c>
+      <c r="F35" s="1">
+        <v>6.3868</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F37" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>